<commit_message>
server_send 완성, DB-table 설계중
</commit_message>
<xml_diff>
--- a/blueprint/table_design.xlsx
+++ b/blueprint/table_design.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\ARK\Git\mini_pot\blueprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4075B066-81A6-46E1-9F31-A3B1557F2A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4379C6-197E-442A-8EEF-4BFD935F8EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10125" yWindow="1725" windowWidth="17235" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8565" yWindow="4020" windowWidth="17235" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="52">
   <si>
     <t>생장정보</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -67,10 +76,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>&lt; my account &gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -79,7 +84,153 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>(회원번호)</t>
+    <t>PW : 8~16자 영문 대 소문자, 숫자, 특수문자를 사용하세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID : 5~20자의 영문 대 소문자, 숫자와 특수기호(_),(-)만 사용 가능합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">E-mail : 6글자 이상, @ 필수 </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt; plant_guide &gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>( server : 식물 생장정보 )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>식별번호</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>식물이름</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최저온도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최고온도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최저습도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최고습도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최저빛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최고빛</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최저영양액</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최고영양액</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Rpi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>plant</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>temp1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>temp2</t>
+  </si>
+  <si>
+    <t>temp3</t>
+  </si>
+  <si>
+    <t>ABC001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ABC002</t>
+  </si>
+  <si>
+    <t>ABC003</t>
+  </si>
+  <si>
+    <t>q1w2e3r4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>w2e3r4t5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e3r4t5y6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt; account &gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>( server : 회원정보 )</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>no</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A002</t>
+  </si>
+  <si>
+    <t>A003</t>
+  </si>
+  <si>
+    <t>i1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>i2</t>
+  </si>
+  <si>
+    <t>i3</t>
+  </si>
+  <si>
+    <t>PW : 해쉬 알고리즘 사용해야함 (MD5, SHA1)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -123,9 +274,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -406,31 +558,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G13"/>
+  <dimension ref="B2:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="3" max="3" width="10.25" customWidth="1"/>
+    <col min="9" max="9" width="13.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -449,8 +609,41 @@
       <c r="G6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" t="s">
+        <v>19</v>
+      </c>
+      <c r="L6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M6" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" t="s">
+        <v>22</v>
+      </c>
+      <c r="O6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>25</v>
+      </c>
+      <c r="R6" t="s">
+        <v>26</v>
+      </c>
+      <c r="S6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B7" s="1">
         <v>36547.473993055559</v>
       </c>
@@ -469,8 +662,41 @@
       <c r="G7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="I7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J7" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7">
+        <v>10</v>
+      </c>
+      <c r="L7">
+        <v>20</v>
+      </c>
+      <c r="M7">
+        <v>30</v>
+      </c>
+      <c r="N7">
+        <v>40</v>
+      </c>
+      <c r="O7">
+        <v>50</v>
+      </c>
+      <c r="P7">
+        <v>60</v>
+      </c>
+      <c r="Q7">
+        <v>70</v>
+      </c>
+      <c r="R7">
+        <v>80</v>
+      </c>
+      <c r="S7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B8" s="1">
         <v>36548.474120370367</v>
       </c>
@@ -486,8 +712,44 @@
       <c r="F8">
         <v>56.78</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8">
+        <v>11</v>
+      </c>
+      <c r="L8">
+        <v>22</v>
+      </c>
+      <c r="M8">
+        <v>33</v>
+      </c>
+      <c r="N8">
+        <v>44</v>
+      </c>
+      <c r="O8">
+        <v>55</v>
+      </c>
+      <c r="P8">
+        <v>66</v>
+      </c>
+      <c r="Q8">
+        <v>77</v>
+      </c>
+      <c r="R8">
+        <v>88</v>
+      </c>
+      <c r="S8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
       <c r="B9" s="1">
         <v>36549.474247685182</v>
       </c>
@@ -503,41 +765,222 @@
       <c r="F9">
         <v>56.78</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="1">
-        <v>36550.474259259259</v>
+      <c r="G9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9">
+        <v>100</v>
+      </c>
+      <c r="L9">
+        <v>200</v>
+      </c>
+      <c r="M9">
+        <v>300</v>
+      </c>
+      <c r="N9">
+        <v>400</v>
+      </c>
+      <c r="O9">
+        <v>500</v>
+      </c>
+      <c r="P9">
+        <v>600</v>
+      </c>
+      <c r="Q9">
+        <v>700</v>
+      </c>
+      <c r="R9">
+        <v>800</v>
+      </c>
+      <c r="S9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" t="s">
+        <v>29</v>
+      </c>
+      <c r="J10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" t="s">
+        <v>29</v>
+      </c>
+      <c r="L10" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" t="s">
+        <v>29</v>
+      </c>
+      <c r="N10" t="s">
+        <v>29</v>
+      </c>
+      <c r="O10" t="s">
+        <v>29</v>
+      </c>
+      <c r="P10" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>29</v>
+      </c>
+      <c r="R10" t="s">
+        <v>29</v>
+      </c>
+      <c r="S10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" t="s">
+        <v>32</v>
+      </c>
+      <c r="G16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
         <v>12</v>
       </c>
-      <c r="E10">
-        <v>34</v>
-      </c>
-      <c r="F10">
-        <v>56.78</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" t="s">
-        <v>2</v>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>